<commit_message>
TowerProjectile, TowerHitEffct 구현 현재 타워는 총 4개(기본타워, 불,물,전기)
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Data/ExcelData/GameEntityData.xlsx
+++ b/Assets/Scripts/Data/ExcelData/GameEntityData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t>dataID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -321,6 +321,26 @@
   </si>
   <si>
     <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>towerTypePath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/NormarTowerType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/FireTowerType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/LightTowerType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/IceTowerType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -651,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -662,9 +682,10 @@
     <col min="2" max="2" width="14.125" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
     <col min="5" max="5" width="33.875" customWidth="1"/>
+    <col min="6" max="6" width="27.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -680,8 +701,11 @@
       <c r="E1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -694,8 +718,11 @@
       <c r="E2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -708,8 +735,11 @@
       <c r="E3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -722,8 +752,11 @@
       <c r="E4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -736,8 +769,11 @@
       <c r="E5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -750,8 +786,11 @@
       <c r="E6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -764,8 +803,11 @@
       <c r="E7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -778,8 +820,11 @@
       <c r="E8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -792,8 +837,11 @@
       <c r="E9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -806,8 +854,11 @@
       <c r="E10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -820,8 +871,11 @@
       <c r="E11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -834,8 +888,11 @@
       <c r="E12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -848,8 +905,11 @@
       <c r="E13" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -859,11 +919,8 @@
       <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="E14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -874,7 +931,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -930,7 +987,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
StagePanelUI, PlayerPanelUI 수정, 디텍터 수정(제네릭사용)
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Data/ExcelData/GameEntityData.xlsx
+++ b/Assets/Scripts/Data/ExcelData/GameEntityData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TowerDefence\Assets\Scripts\Data\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOON\TowerDefence\Assets\Scripts\Data\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D11E79-5943-4294-AB5B-BF616A56CD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="profileEntity" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
   <si>
     <t>dataID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,318 +41,345 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackDamage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rotationSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nor33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normon11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normon12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>normon13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bosmon11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bosmon12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bosmon13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노말몬스터1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노말몬스터2</t>
+  </si>
+  <si>
+    <t>노말몬스터3</t>
+  </si>
+  <si>
+    <t>보스몬스터1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보스몬스터2</t>
+  </si>
+  <si>
+    <t>보스몬스터3</t>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NormarTower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NormarMonster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BossMonster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/Normar/LV1_Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/Normar/LV2_Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/Normar/LV3_Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/Boss/LV1_Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/Boss/LV2_Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/Boss/LV3_Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/LV1_Golem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/FireTower1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/FireTower2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/FireTower3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하급불타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중급불타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고급불타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하급얼음타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중급얼음타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고급얼음타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하급전기타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중급전기타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고급전기타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/IceTower1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/IceTower2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/IceTower3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/LightTower1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/LightTower2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/LightTower3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Tower/Character/MortarTower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하급총알타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중급총알타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고급총알타워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Projectile/FireProjectile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Projectile/IceProjectile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Projectile/LightningProjectile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>projectilePath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Projectile/TowerProjectile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>towerTypePath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/NormarTowerType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/FireTowerType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/LightTowerType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/IceTowerType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spawnCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>iconPath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attackDamage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attackSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rotationSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor21</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor22</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor23</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor32</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nor33</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>attackRange</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>normon11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>normon12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>normon13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bosmon11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bosmon12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bosmon13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>노말몬스터1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>노말몬스터2</t>
-  </si>
-  <si>
-    <t>노말몬스터3</t>
-  </si>
-  <si>
-    <t>보스몬스터1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>보스몬스터2</t>
-  </si>
-  <si>
-    <t>보스몬스터3</t>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NormarTower</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NormarMonster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BossMonster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>moveSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>coin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Monster/Normar/LV1_Golem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Monster/Normar/LV2_Golem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Monster/Normar/LV3_Golem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Monster/Boss/LV1_Golem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Monster/Boss/LV2_Golem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Monster/Boss/LV3_Golem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Monster/LV1_Golem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/FireTower1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/FireTower2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/FireTower3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하급불타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중급불타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고급불타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하급얼음타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중급얼음타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고급얼음타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하급전기타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중급전기타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고급전기타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/IceTower1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/IceTower2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/IceTower3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/LightTower1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/LightTower2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/LightTower3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Tower/Character/MortarTower</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>하급총알타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중급총알타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고급총알타워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Projectile/FireProjectile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Projectile/IceProjectile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Projectile/LightningProjectile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>projectilePath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Projectile/TowerProjectile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>level</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>towerTypePath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconImage/NormarTowerType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconImage/FireTowerType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconImage/LightTowerType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconImage/IceTowerType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spawnCount</t>
+  </si>
+  <si>
+    <t>monsterHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/Normar1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconImage/Normar2</t>
+  </si>
+  <si>
+    <t>IconImage/Normar3</t>
+  </si>
+  <si>
+    <t>IconImage/Boss2</t>
+  </si>
+  <si>
+    <t>IconImage/Boss3</t>
+  </si>
+  <si>
+    <t>IconImage/Boss1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rewardCoin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iconPath</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -676,19 +702,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.125" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="5" max="5" width="33.875" customWidth="1"/>
-    <col min="6" max="6" width="27.875" customWidth="1"/>
+    <col min="4" max="4" width="33.875" customWidth="1"/>
+    <col min="5" max="5" width="27.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -702,283 +728,283 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -989,7 +1015,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1009,30 +1035,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1000</v>
@@ -1050,7 +1076,7 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1058,7 +1084,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>2000</v>
@@ -1076,7 +1102,7 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -1084,7 +1110,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>3000</v>
@@ -1102,7 +1128,7 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -1110,7 +1136,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -1128,7 +1154,7 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1136,7 +1162,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>2000</v>
@@ -1154,7 +1180,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -1162,7 +1188,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>3000</v>
@@ -1180,7 +1206,7 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -1188,7 +1214,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>1000</v>
@@ -1206,7 +1232,7 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1214,7 +1240,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>2000</v>
@@ -1232,7 +1258,7 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -1240,7 +1266,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>3000</v>
@@ -1258,7 +1284,7 @@
         <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10">
         <v>3</v>
@@ -1266,7 +1292,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>1000</v>
@@ -1284,7 +1310,7 @@
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1292,7 +1318,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>2000</v>
@@ -1310,7 +1336,7 @@
         <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12">
         <v>2</v>
@@ -1318,7 +1344,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>3000</v>
@@ -1336,7 +1362,7 @@
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13">
         <v>3</v>
@@ -1350,11 +1376,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1363,6 +1389,7 @@
     <col min="3" max="3" width="17.375" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="15.75" customWidth="1"/>
+    <col min="7" max="7" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1370,27 +1397,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>150</v>
@@ -1402,7 +1429,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1413,7 +1440,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>300</v>
@@ -1425,7 +1452,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1436,7 +1463,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>450</v>
@@ -1448,7 +1475,7 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -1459,7 +1486,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>1500</v>
@@ -1471,7 +1498,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1482,7 +1509,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>3000</v>
@@ -1494,7 +1521,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -1505,7 +1532,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>4500</v>
@@ -1517,7 +1544,7 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -1534,11 +1561,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1546,104 +1573,170 @@
     <col min="2" max="2" width="13.625" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="27.625" customWidth="1"/>
+    <col min="6" max="6" width="13.25" customWidth="1"/>
+    <col min="7" max="8" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2">
+        <v>150</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4">
+        <v>450</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5">
+        <v>1500</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6">
+        <v>3000</v>
+      </c>
+      <c r="G6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7">
+        <v>4500</v>
+      </c>
+      <c r="G7">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>